<commit_message>
Added files required for foam run. Got command line functionality working with argparse.
</commit_message>
<xml_diff>
--- a/stovegeom/Stove_Geometry.xlsx
+++ b/stovegeom/Stove_Geometry.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Oregon_State\Spring 2019\Soft_dev_eng\Project\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Oregon_State\Spring_2019\Soft_dev_eng\StoveOpt\stovegeom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1293FA7D-C438-4CBD-9E47-18A6E14F5DDC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3745C4-C49D-45EE-AEA2-34B387DCDDCD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4272" yWindow="0" windowWidth="17280" windowHeight="8964" activeTab="3" xr2:uid="{D0F77571-F344-4911-9ED7-19CABFB8BC85}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{D0F77571-F344-4911-9ED7-19CABFB8BC85}"/>
   </bookViews>
   <sheets>
     <sheet name="Purpose" sheetId="1" r:id="rId1"/>
@@ -178,6 +178,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.00000000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -230,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -239,6 +242,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -340,7 +346,7 @@
             <c:numRef>
               <c:f>Outputs!$C$2:$C$17</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00000000</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -397,7 +403,7 @@
             <c:numRef>
               <c:f>Outputs!$D$2:$D$17</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00000000</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -489,7 +495,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00000000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -551,7 +557,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00000000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2672,8 +2678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F96E3B86-B810-49F2-ADC9-6B1B0C4097E0}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2712,15 +2718,15 @@
       <c r="B2" s="3">
         <v>1</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4">
         <f>Intermediate!C2*(1/100)</f>
         <v>0</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="4">
         <f>Intermediate!D2*(1/100)</f>
         <v>0</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="4">
         <f>Intermediate!E2*(1/100)</f>
         <v>0</v>
       </c>
@@ -2735,15 +2741,15 @@
       <c r="B3" s="3">
         <v>2</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="4">
         <f>Intermediate!C3*(1/100)</f>
         <v>0.1</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="4">
         <f>Intermediate!D3*(1/100)</f>
         <v>0</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="4">
         <f>Intermediate!E3*(1/100)</f>
         <v>0</v>
       </c>
@@ -2758,15 +2764,15 @@
       <c r="B4" s="3">
         <v>3</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="4">
         <f>Intermediate!C4*(1/100)</f>
         <v>0</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="4">
         <f>Intermediate!D4*(1/100)</f>
         <v>0.15</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="4">
         <f>Intermediate!E4*(1/100)</f>
         <v>0</v>
       </c>
@@ -2781,15 +2787,15 @@
       <c r="B5" s="3">
         <v>4</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="4">
         <f>Intermediate!C5*(1/100)</f>
         <v>0.1</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="4">
         <f>Intermediate!D5*(1/100)</f>
         <v>0.15</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="4">
         <f>Intermediate!E5*(1/100)</f>
         <v>0</v>
       </c>
@@ -2804,15 +2810,15 @@
       <c r="B6" s="3">
         <v>5</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="4">
         <f>Intermediate!C6*(1/100)</f>
         <v>0.1</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="4">
         <f>Intermediate!D6*(1/100)</f>
         <v>0.16</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="4">
         <f>Intermediate!E6*(1/100)</f>
         <v>0</v>
       </c>
@@ -2827,15 +2833,15 @@
       <c r="B7" s="3">
         <v>6</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="4">
         <f>Intermediate!C7*(1/100)</f>
         <v>0</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="4">
         <f>Intermediate!D7*(1/100)</f>
         <v>0.16</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="4">
         <f>Intermediate!E7*(1/100)</f>
         <v>0</v>
       </c>
@@ -2850,15 +2856,15 @@
       <c r="B8" s="3">
         <v>7</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="4">
         <f>Intermediate!C8*(1/100)</f>
         <v>0</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="4">
         <f>Intermediate!D8*(1/100)</f>
         <v>0.3</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="4">
         <f>Intermediate!E8*(1/100)</f>
         <v>0</v>
       </c>
@@ -2873,15 +2879,15 @@
       <c r="B9" s="3">
         <v>8</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="4">
         <f>Intermediate!C9*(1/100)</f>
         <v>0.1</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="4">
         <f>Intermediate!D9*(1/100)</f>
         <v>0.3</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="4">
         <f>Intermediate!E9*(1/100)</f>
         <v>0</v>
       </c>
@@ -2896,15 +2902,15 @@
       <c r="B10" s="3">
         <v>9</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="4">
         <f>Intermediate!C10*(1/100)</f>
         <v>0.17</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="4">
         <f>Intermediate!D10*(1/100)</f>
         <v>0.3</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="4">
         <f>Intermediate!E10*(1/100)</f>
         <v>0</v>
       </c>
@@ -2919,15 +2925,15 @@
       <c r="B11" s="3">
         <v>10</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="4">
         <f>Intermediate!C11*(1/100)</f>
         <v>-7.0000000000000007E-2</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="4">
         <f>Intermediate!D11*(1/100)</f>
         <v>0.3</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="4">
         <f>Intermediate!E11*(1/100)</f>
         <v>0</v>
       </c>
@@ -2942,15 +2948,15 @@
       <c r="B12" s="3">
         <v>11</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="4">
         <f>Intermediate!C12*(1/100)</f>
         <v>-7.0000000000000007E-2</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="4">
         <f>Intermediate!D12*(1/100)</f>
         <v>0.5</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="4">
         <f>Intermediate!E12*(1/100)</f>
         <v>0</v>
       </c>
@@ -2965,15 +2971,15 @@
       <c r="B13" s="3">
         <v>12</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="4">
         <f>Intermediate!C13*(1/100)</f>
         <v>-0.04</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="4">
         <f>Intermediate!D13*(1/100)</f>
         <v>0.5</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="4">
         <f>Intermediate!E13*(1/100)</f>
         <v>0</v>
       </c>
@@ -2988,15 +2994,15 @@
       <c r="B14" s="3">
         <v>13</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="4">
         <f>Intermediate!C14*(1/100)</f>
         <v>0.14000000000000001</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="4">
         <f>Intermediate!D14*(1/100)</f>
         <v>0.5</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="4">
         <f>Intermediate!E14*(1/100)</f>
         <v>0</v>
       </c>
@@ -3011,15 +3017,15 @@
       <c r="B15" s="3">
         <v>14</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="4">
         <f>Intermediate!C15*(1/100)</f>
         <v>0.17</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="4">
         <f>Intermediate!D15*(1/100)</f>
         <v>0.5</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="4">
         <f>Intermediate!E15*(1/100)</f>
         <v>0</v>
       </c>
@@ -3034,15 +3040,15 @@
       <c r="B16" s="3">
         <v>15</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="4">
         <f>Intermediate!C16*(1/100)</f>
         <v>-0.04</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="4">
         <f>Intermediate!D16*(1/100)</f>
         <v>0.33</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="4">
         <f>Intermediate!E16*(1/100)</f>
         <v>0</v>
       </c>
@@ -3057,15 +3063,15 @@
       <c r="B17" s="3">
         <v>16</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="4">
         <f>Intermediate!C17*(1/100)</f>
         <v>0.14000000000000001</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="4">
         <f>Intermediate!D17*(1/100)</f>
         <v>0.33</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="4">
         <f>Intermediate!E17*(1/100)</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Tested and verified functionality for writing geometry to meshing procedure for OpenFoam. Next, writing functionality for assigning boundary conditions
</commit_message>
<xml_diff>
--- a/stovegeom/Stove_Geometry.xlsx
+++ b/stovegeom/Stove_Geometry.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Oregon_State\Spring_2019\Soft_dev_eng\StoveOpt\stovegeom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3745C4-C49D-45EE-AEA2-34B387DCDDCD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFEEFDB1-6640-43D1-89EA-A4C4438C45F2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{D0F77571-F344-4911-9ED7-19CABFB8BC85}"/>
   </bookViews>
@@ -179,7 +179,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.00000000"/>
+    <numFmt numFmtId="164" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -244,7 +244,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1577,16 +1577,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>693420</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1193722</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>137929</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>792480</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>299873</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>29402</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2678,8 +2678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F96E3B86-B810-49F2-ADC9-6B1B0C4097E0}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2716,7 +2716,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="4">
         <f>Intermediate!C2*(1/100)</f>
@@ -2739,7 +2739,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="4">
         <f>Intermediate!C3*(1/100)</f>
@@ -2762,7 +2762,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="4">
         <f>Intermediate!C4*(1/100)</f>
@@ -2785,7 +2785,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="4">
         <f>Intermediate!C5*(1/100)</f>
@@ -2808,7 +2808,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="4">
         <f>Intermediate!C6*(1/100)</f>
@@ -2831,7 +2831,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="4">
         <f>Intermediate!C7*(1/100)</f>
@@ -2854,7 +2854,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="4">
         <f>Intermediate!C8*(1/100)</f>
@@ -2877,7 +2877,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="4">
         <f>Intermediate!C9*(1/100)</f>
@@ -2900,7 +2900,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="4">
         <f>Intermediate!C10*(1/100)</f>
@@ -2923,7 +2923,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="4">
         <f>Intermediate!C11*(1/100)</f>
@@ -2946,7 +2946,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="3">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="4">
         <f>Intermediate!C12*(1/100)</f>
@@ -2969,7 +2969,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="3">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="4">
         <f>Intermediate!C13*(1/100)</f>
@@ -2992,7 +2992,7 @@
         <v>37</v>
       </c>
       <c r="B14" s="3">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="4">
         <f>Intermediate!C14*(1/100)</f>
@@ -3015,7 +3015,7 @@
         <v>38</v>
       </c>
       <c r="B15" s="3">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" s="4">
         <f>Intermediate!C15*(1/100)</f>
@@ -3038,7 +3038,7 @@
         <v>44</v>
       </c>
       <c r="B16" s="3">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="4">
         <f>Intermediate!C16*(1/100)</f>
@@ -3061,7 +3061,7 @@
         <v>45</v>
       </c>
       <c r="B17" s="3">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="4">
         <f>Intermediate!C17*(1/100)</f>

</xml_diff>

<commit_message>
added postprocessing and new simulation setups
</commit_message>
<xml_diff>
--- a/stovegeom/Stove_Geometry.xlsx
+++ b/stovegeom/Stove_Geometry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Oregon_State\Spring_2019\Soft_dev_eng\StoveOpt\stovegeom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFEEFDB1-6640-43D1-89EA-A4C4438C45F2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E45145-4905-46B1-88DE-A10936C69306}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{D0F77571-F344-4911-9ED7-19CABFB8BC85}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{D0F77571-F344-4911-9ED7-19CABFB8BC85}"/>
   </bookViews>
   <sheets>
     <sheet name="Purpose" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="53">
   <si>
     <t>Geometry</t>
   </si>
@@ -172,6 +172,27 @@
   </si>
   <si>
     <t>RHS bottom inner channel wall</t>
+  </si>
+  <si>
+    <t>Qs</t>
+  </si>
+  <si>
+    <t>Flow Definition</t>
+  </si>
+  <si>
+    <t>Secondary air flow rate</t>
+  </si>
+  <si>
+    <t>m2/s</t>
+  </si>
+  <si>
+    <t>U_100</t>
+  </si>
+  <si>
+    <t>Primary air flow rate</t>
+  </si>
+  <si>
+    <t>Qp</t>
   </si>
 </sst>
 </file>
@@ -206,7 +227,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -229,11 +250,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -245,6 +279,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1928,8 +1971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADDE5443-8426-4515-AD7B-44481396F926}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2103,19 +2146,46 @@
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+      <c r="A13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="A14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+      <c r="A15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
@@ -2678,8 +2748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F96E3B86-B810-49F2-ADC9-6B1B0C4097E0}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:B17"/>
+    <sheetView topLeftCell="B1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2692,7 +2762,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -2712,7 +2782,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="3">
@@ -2735,7 +2805,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="3">
@@ -2758,7 +2828,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="3">
@@ -2781,7 +2851,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="3">
@@ -2804,7 +2874,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="3">
@@ -2827,7 +2897,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="3">
@@ -2850,7 +2920,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B8" s="3">
@@ -2873,7 +2943,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B9" s="3">
@@ -2896,7 +2966,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B10" s="3">
@@ -2919,7 +2989,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="3">
@@ -2942,7 +3012,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B12" s="3">
@@ -2965,7 +3035,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B13" s="3">
@@ -2988,7 +3058,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="7" t="s">
         <v>37</v>
       </c>
       <c r="B14" s="3">
@@ -3011,7 +3081,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B15" s="3">
@@ -3034,7 +3104,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="7" t="s">
         <v>44</v>
       </c>
       <c r="B16" s="3">
@@ -3057,7 +3127,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="7" t="s">
         <v>45</v>
       </c>
       <c r="B17" s="3">
@@ -3081,11 +3151,22 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="B18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="3">
+        <f>ABS(Inputs!C14)</f>
+        <v>1</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>

</xml_diff>

<commit_message>
adding files to github to test on faster machine
</commit_message>
<xml_diff>
--- a/stovegeom/Stove_Geometry.xlsx
+++ b/stovegeom/Stove_Geometry.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Oregon_State\Spring_2019\Soft_dev_eng\StoveOpt\stovegeom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E45145-4905-46B1-88DE-A10936C69306}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58EF2EC8-51F0-40BC-9005-BA0BECEB5B09}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{D0F77571-F344-4911-9ED7-19CABFB8BC85}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{D0F77571-F344-4911-9ED7-19CABFB8BC85}"/>
   </bookViews>
   <sheets>
     <sheet name="Purpose" sheetId="1" r:id="rId1"/>
     <sheet name="Inputs" sheetId="2" r:id="rId2"/>
     <sheet name="Intermediate" sheetId="4" r:id="rId3"/>
-    <sheet name="Outputs" sheetId="3" r:id="rId4"/>
+    <sheet name="Intermediate 2" sheetId="5" r:id="rId4"/>
+    <sheet name="Outputs" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="72">
   <si>
     <t>Geometry</t>
   </si>
@@ -193,6 +194,84 @@
   </si>
   <si>
     <t>Qp</t>
+  </si>
+  <si>
+    <t>Area of the secondary inlet</t>
+  </si>
+  <si>
+    <t>Bulk flow velocity</t>
+  </si>
+  <si>
+    <t>flow rate (m2/s)</t>
+  </si>
+  <si>
+    <t>Diameter secondary inlet</t>
+  </si>
+  <si>
+    <t>area secondary air inlet</t>
+  </si>
+  <si>
+    <t>m^2</t>
+  </si>
+  <si>
+    <t>bulk flow velocity</t>
+  </si>
+  <si>
+    <t>m/s</t>
+  </si>
+  <si>
+    <t>Flow rate</t>
+  </si>
+  <si>
+    <t>m^3/s</t>
+  </si>
+  <si>
+    <t>mass flux</t>
+  </si>
+  <si>
+    <t>density air</t>
+  </si>
+  <si>
+    <t>kg/m3</t>
+  </si>
+  <si>
+    <t>ks/s</t>
+  </si>
+  <si>
+    <r>
+      <t>2.0 m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/min</t>
+    </r>
+  </si>
+  <si>
+    <t>computer fan flow rate</t>
+  </si>
+  <si>
+    <t>m3/min</t>
+  </si>
+  <si>
+    <t>computer fan flow rate corr</t>
+  </si>
+  <si>
+    <t>m3/s</t>
   </si>
 </sst>
 </file>
@@ -202,7 +281,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,6 +296,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="7"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -267,7 +359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -290,6 +382,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1971,8 +2067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADDE5443-8426-4515-AD7B-44481396F926}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2167,7 +2263,7 @@
         <v>46</v>
       </c>
       <c r="C14" s="3">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>49</v>
@@ -2258,7 +2354,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:B17"/>
+      <selection sqref="A1:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2650,7 +2746,9 @@
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -2674,16 +2772,26 @@
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
+      <c r="A22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
+      <c r="A23" s="1">
+        <f>(PI()/4)*((D6/100)-(D5/100))^2</f>
+        <v>7.8539816339744976E-5</v>
+      </c>
+      <c r="B23" s="1">
+        <f>Inputs!C14/Intermediate!A23</f>
+        <v>1273.2395447351605</v>
+      </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -2745,11 +2853,526 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51B2D988-8AA1-459C-82C6-62AF672456D7}">
+  <dimension ref="A1:F29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="37" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="19.77734375" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <f>Intermediate!C2/100</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <f>Intermediate!D2/100</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <f>Intermediate!E2/100</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3">
+        <f>Intermediate!C3/100</f>
+        <v>0.1</v>
+      </c>
+      <c r="D3" s="3">
+        <f>Intermediate!D3/100</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="3">
+        <f>Intermediate!E3/100</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="3">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3">
+        <f>Intermediate!C4/100</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <f>Intermediate!D4/100</f>
+        <v>0.15</v>
+      </c>
+      <c r="E4" s="3">
+        <f>Intermediate!E4/100</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="3">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3">
+        <f>Intermediate!C5/100</f>
+        <v>0.1</v>
+      </c>
+      <c r="D5" s="3">
+        <f>Intermediate!D5/100</f>
+        <v>0.15</v>
+      </c>
+      <c r="E5" s="3">
+        <f>Intermediate!E5/100</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="3">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3">
+        <f>Intermediate!C6/100</f>
+        <v>0.1</v>
+      </c>
+      <c r="D6" s="3">
+        <f>Intermediate!D6/100</f>
+        <v>0.16</v>
+      </c>
+      <c r="E6" s="3">
+        <f>Intermediate!E6/100</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3">
+        <f>Intermediate!C7/100</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="3">
+        <f>Intermediate!D7/100</f>
+        <v>0.16</v>
+      </c>
+      <c r="E7" s="3">
+        <f>Intermediate!E7/100</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="3">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3">
+        <f>Intermediate!C8/100</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <f>Intermediate!D8/100</f>
+        <v>0.3</v>
+      </c>
+      <c r="E8" s="3">
+        <f>Intermediate!E8/100</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="3">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3">
+        <f>Intermediate!C9/100</f>
+        <v>0.1</v>
+      </c>
+      <c r="D9" s="3">
+        <f>Intermediate!D9/100</f>
+        <v>0.3</v>
+      </c>
+      <c r="E9" s="3">
+        <f>Intermediate!E9/100</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="3">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3">
+        <f>Intermediate!C10/100</f>
+        <v>0.17</v>
+      </c>
+      <c r="D10" s="3">
+        <f>Intermediate!D10/100</f>
+        <v>0.3</v>
+      </c>
+      <c r="E10" s="3">
+        <f>Intermediate!E10/100</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="3">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3">
+        <f>Intermediate!C11/100</f>
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="D11" s="3">
+        <f>Intermediate!D11/100</f>
+        <v>0.3</v>
+      </c>
+      <c r="E11" s="3">
+        <f>Intermediate!E11/100</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="3">
+        <v>11</v>
+      </c>
+      <c r="C12" s="3">
+        <f>Intermediate!C12/100</f>
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="D12" s="3">
+        <f>Intermediate!D12/100</f>
+        <v>0.5</v>
+      </c>
+      <c r="E12" s="3">
+        <f>Intermediate!E12/100</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="3">
+        <v>12</v>
+      </c>
+      <c r="C13" s="3">
+        <f>Intermediate!C13/100</f>
+        <v>-0.04</v>
+      </c>
+      <c r="D13" s="3">
+        <f>Intermediate!D13/100</f>
+        <v>0.5</v>
+      </c>
+      <c r="E13" s="3">
+        <f>Intermediate!E13/100</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="3">
+        <v>13</v>
+      </c>
+      <c r="C14" s="3">
+        <f>Intermediate!C14/100</f>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D14" s="3">
+        <f>Intermediate!D14/100</f>
+        <v>0.5</v>
+      </c>
+      <c r="E14" s="3">
+        <f>Intermediate!E14/100</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="3">
+        <v>14</v>
+      </c>
+      <c r="C15" s="3">
+        <f>Intermediate!C15/100</f>
+        <v>0.17</v>
+      </c>
+      <c r="D15" s="3">
+        <f>Intermediate!D15/100</f>
+        <v>0.5</v>
+      </c>
+      <c r="E15" s="3">
+        <f>Intermediate!E15/100</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="3">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3">
+        <f>Intermediate!C16/100</f>
+        <v>-0.04</v>
+      </c>
+      <c r="D16" s="3">
+        <f>Intermediate!D16/100</f>
+        <v>0.33</v>
+      </c>
+      <c r="E16" s="3">
+        <f>Intermediate!E16/100</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="3">
+        <v>16</v>
+      </c>
+      <c r="C17" s="3">
+        <f>Intermediate!C17/100</f>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D17" s="3">
+        <f>Intermediate!D17/100</f>
+        <v>0.33</v>
+      </c>
+      <c r="E17" s="3">
+        <f>Intermediate!E17/100</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="1">
+        <f>D6-D5</f>
+        <v>1.0000000000000009E-2</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="1">
+        <f>(PI()/4)*B20^2</f>
+        <v>7.8539816339744976E-5</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="1">
+        <v>318.30988618379001</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="1">
+        <f>B22*B21</f>
+        <v>2.4999999999999994E-2</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="1">
+        <f>1.225</f>
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="1">
+        <f>B24*B23</f>
+        <v>3.0624999999999996E-2</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="1">
+        <f>2</f>
+        <v>2</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="1">
+        <f>B28/60</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F96E3B86-B810-49F2-ADC9-6B1B0C4097E0}">
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3156,7 +3779,7 @@
       </c>
       <c r="C18" s="3">
         <f>ABS(Inputs!C14)</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D18" s="3">
         <v>0</v>

</xml_diff>